<commit_message>
actualización de bovino y agricultura
</commit_message>
<xml_diff>
--- a/docs/source/recursos/agricultura/tabla_cat_fv_agtem_bio_prec_precipitacion.xlsx
+++ b/docs/source/recursos/agricultura/tabla_cat_fv_agtem_bio_prec_precipitacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox (LANCIS)\FOMIX\fmx_estudio_tecnico\diagnostico\talleres\sphinx\docs\source\recursos\agricultura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3A61837-D9FF-46D3-A438-8C7EB94EA5BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0809ECEC-FAB8-4C2B-9DA2-9462992017A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F879907D-B976-4D78-92BE-EAAFE967E4C3}"/>
   </bookViews>
@@ -38,43 +38,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
-    <t>a) 551-626 mm</t>
-  </si>
-  <si>
     <t>Baja</t>
   </si>
   <si>
-    <t>b) 626-778 mm</t>
-  </si>
-  <si>
-    <t>c) 778-930 mm</t>
-  </si>
-  <si>
     <t>Moderada</t>
   </si>
   <si>
-    <t>d) 930-1081 mm</t>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
-    <t>e) 1081-1233 mm</t>
-  </si>
-  <si>
     <t>Muy alta</t>
   </si>
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Categoría</t>
-  </si>
-  <si>
     <t>Importancia</t>
   </si>
   <si>
     <t>FV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">626-778 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">551-626 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">778-930 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">930-1081 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1081-1233 </t>
+  </si>
+  <si>
+    <t>Categoría (mm)</t>
   </si>
 </sst>
 </file>
@@ -146,7 +146,7 @@
       <sheetName val="clasificacion"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="A1" t="str">
@@ -511,23 +511,23 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -535,10 +535,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3">
         <f>VLOOKUP(C2,[1]clasificacion!$A$1:$C$6,3,FALSE)</f>
@@ -550,10 +550,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3">
         <f>VLOOKUP(C3,[1]clasificacion!$A$1:$C$6,3,FALSE)</f>
@@ -565,10 +565,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3">
         <f>VLOOKUP(C4,[1]clasificacion!$A$1:$C$6,3,FALSE)</f>
@@ -577,13 +577,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="D5" s="3">
         <f>VLOOKUP(C5,[1]clasificacion!$A$1:$C$6,3,FALSE)</f>
@@ -592,13 +592,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
         <f>VLOOKUP(C6,[1]clasificacion!$A$1:$C$6,3,FALSE)</f>
@@ -606,8 +606,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D6">
-    <sortCondition descending="1" ref="D2:D6"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D5">
+    <sortCondition descending="1" ref="D2:D5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -617,7 +617,7 @@
           <x14:formula1>
             <xm:f>'C:\Dropbox (LANCIS)\FOMIX\fmx_estudio_tecnico\diagnostico\talleres\sectores\agricultura\funciones_valor\[tabla_tabla_fv_agtem_bio_prec_precipitacion.xlsm]clasificacion'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C6</xm:sqref>
+          <xm:sqref>C2:C4 C5:C6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>